<commit_message>
Revert "Revert "Update author.xlsx""
This reverts commit 2e47f214a4b6cf41ad482f09a80ed3f4db6d1979.
</commit_message>
<xml_diff>
--- a/author.xlsx
+++ b/author.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9511CC-7C48-4D07-A139-FC0A90E5C1F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74AC74FB-723C-4E10-83D8-709DF7403831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="56">
   <si>
     <t>Short Description</t>
   </si>
@@ -189,6 +189,9 @@
   </si>
   <si>
     <t>puli193</t>
+  </si>
+  <si>
+    <t>Maschinenbau und Design</t>
   </si>
 </sst>
 </file>
@@ -851,14 +854,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F9303FD-2881-47EE-8AD0-19738A635E19}">
   <dimension ref="A2:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="47.36328125" customWidth="1"/>
-    <col min="2" max="2" width="18.453125" customWidth="1"/>
+    <col min="2" max="2" width="31.26953125" customWidth="1"/>
     <col min="3" max="3" width="33.08984375" customWidth="1"/>
     <col min="4" max="4" width="15.36328125" bestFit="1" customWidth="1"/>
   </cols>
@@ -930,6 +933,9 @@
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>